<commit_message>
Fix the data out enable signal for TX and doc
</commit_message>
<xml_diff>
--- a/doc/SDIO_reference.xlsx
+++ b/doc/SDIO_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -857,12 +857,6 @@
     <t xml:space="preserve">TX_SIZE</t>
   </si>
   <si>
-    <t xml:space="preserve">CMD_OP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO command opcode</t>
-  </si>
-  <si>
     <t xml:space="preserve">CMD_RSP_TYPE</t>
   </si>
   <si>
@@ -872,6 +866,12 @@
 -3’b010: 48 bits no CRC
 -3’b011: 136bits
 -3’b100: 48 bits with BUSY check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO command opcode</t>
   </si>
   <si>
     <t xml:space="preserve">CMD_ARG</t>
@@ -1515,18 +1515,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:D65536"/>
+  <dimension ref="B1:D1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.6632653061225"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="38.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,7 +1774,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1789,16 +1789,16 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="42.9285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="42.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,7 +1815,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1828,18 +1828,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65536"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6173469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="25" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2172,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2186,17 +2187,18 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="43.6020408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="44" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="44" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="44" width="12.9591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="43.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="44" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="44" width="24.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="44" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,7 +2253,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2264,24 +2266,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:53"/>
+  <dimension ref="A1:AMJ53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,7 +3020,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3033,23 +3035,23 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="18.4948979591837"/>
-    <col collapsed="false" hidden="true" max="2" min="2" style="36" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="36" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="25" width="46.1224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="36" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="36" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="36" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="18.49"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="36" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="46.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="36" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="36" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3661,7 +3663,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3674,25 +3676,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="62" width="73.1632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="63" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="62" width="73.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="63" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4137,7 +4139,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
         <v>254</v>
       </c>
@@ -4148,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="44" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E18" s="59" t="s">
         <v>207</v>
@@ -4163,7 +4165,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
         <v>256</v>
       </c>
@@ -4174,7 +4176,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="44" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E19" s="59" t="s">
         <v>207</v>
@@ -4188,6 +4190,7 @@
       <c r="H19" s="67" t="s">
         <v>257</v>
       </c>
+      <c r="J19" s="67"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
@@ -4478,7 +4481,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4493,23 +4496,23 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="63" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="63" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="44" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="44" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="62" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="63" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="63" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="63" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="44" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="44" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="62" width="30.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="63" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4541,7 +4544,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4556,17 +4559,17 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="44" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="76.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="44" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="76.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4589,7 +4592,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4604,19 +4607,19 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="76.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="76.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4642,7 +4645,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add status register for eot, error, and error flag, update document
</commit_message>
<xml_diff>
--- a/doc/SDIO_reference.xlsx
+++ b/doc/SDIO_reference.xlsx
@@ -659,124 +659,100 @@
     <t xml:space="preserve">0x1C</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_CMD_SADDR</t>
+    <t xml:space="preserve">SDIO_CMD_OP</t>
   </si>
   <si>
     <t xml:space="preserve">0x20</t>
   </si>
   <si>
-    <t xml:space="preserve">CMD SDIO uDMA transfer address of associated buffer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_CMD_SIZE</t>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_CMD_ARG</t>
   </si>
   <si>
     <t xml:space="preserve">0x24</t>
   </si>
   <si>
-    <t xml:space="preserve">CMD SDIO uDMA transfer size of buffer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_CMD_CFG</t>
+    <t xml:space="preserve">SDIO argument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_DATA_SETUP</t>
   </si>
   <si>
     <t xml:space="preserve">0x28</t>
   </si>
   <si>
-    <t xml:space="preserve">CMD SDIO uDMA transfer configuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_CMD_INITCFG</t>
+    <t xml:space="preserve">Data transfer setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_START</t>
   </si>
   <si>
     <t xml:space="preserve">0x2C</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO_CMD_OP</t>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_RSP0</t>
   </si>
   <si>
     <t xml:space="preserve">0x30</t>
   </si>
   <si>
-    <t xml:space="preserve">W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO command</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_CMD_ARG</t>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response byte0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_RSP1</t>
   </si>
   <si>
     <t xml:space="preserve">0x34</t>
   </si>
   <si>
-    <t xml:space="preserve">SDIO argument</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_DATA_SETUP</t>
+    <t xml:space="preserve">Response byte1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_RSP2</t>
   </si>
   <si>
     <t xml:space="preserve">0x38</t>
   </si>
   <si>
-    <t xml:space="preserve">Data transfer setup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_START</t>
+    <t xml:space="preserve">Response byte2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_RSP3</t>
   </si>
   <si>
     <t xml:space="preserve">0x3C</t>
   </si>
   <si>
-    <t xml:space="preserve">Start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_RSP0</t>
+    <t xml:space="preserve">Response byte3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_CLK_DIV</t>
   </si>
   <si>
     <t xml:space="preserve">0x40</t>
   </si>
   <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response byte0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_RSP1</t>
+    <t xml:space="preserve">Clock Divider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_STATUS</t>
   </si>
   <si>
     <t xml:space="preserve">0x44</t>
   </si>
   <si>
-    <t xml:space="preserve">Response byte1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_RSP2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response byte2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_RSP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x4C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Response byte3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDIO_CLK_DIV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clock Divider</t>
+    <t xml:space="preserve">STATUS</t>
   </si>
   <si>
     <t xml:space="preserve">Bit field</t>
@@ -928,6 +904,112 @@
   </si>
   <si>
     <t xml:space="preserve">Bytes12..15 of response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EOT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Indicate the end of the transfer of  command or data :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-1'b0: not end
+-1'b1: end</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Indicate the error of the transfer of  command or data :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-1'b0: no error
+-1'b1: error</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_ERR_STATUS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Indicate the error status of the transfer of  command :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-6’b00000: no error
+-6'b00001: Response Time Out
+-6'b00010: Response Wrong Direction
+-6'b00100: Response Busy Timeout</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA_ERR_STATUS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Indicate the error status of the transfer of  data :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">-6’b00000: no error
+-6'b00001: Response Time Out</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Command name</t>
@@ -958,7 +1040,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1010,6 +1092,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1517,16 +1605,16 @@
   </sheetPr>
   <dimension ref="B1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="38.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2284,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="9.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="43.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="44" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="44" width="24.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="44" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="44" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
@@ -2282,7 +2370,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="8.37"/>
   </cols>
   <sheetData>
@@ -3033,12 +3121,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3313,7 +3401,7 @@
       <c r="J9" s="59"/>
       <c r="K9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="36" t="s">
         <v>194</v>
       </c>
@@ -3321,171 +3409,159 @@
         <v>195</v>
       </c>
       <c r="D10" s="36" t="n">
-        <v>32</v>
-      </c>
-      <c r="E10" s="59" t="s">
-        <v>171</v>
+        <v>11</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="59" t="s">
-        <v>170</v>
-      </c>
-      <c r="I10" s="60" t="s">
         <v>196</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>197</v>
       </c>
       <c r="J10" s="61"/>
       <c r="K10" s="61"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D11" s="36" t="n">
         <v>32</v>
       </c>
-      <c r="E11" s="59" t="s">
-        <v>171</v>
-      </c>
       <c r="F11" s="59" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H11" s="59" t="s">
-        <v>170</v>
-      </c>
-      <c r="I11" s="60" t="s">
-        <v>199</v>
+        <v>196</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>200</v>
       </c>
       <c r="J11" s="61"/>
       <c r="K11" s="61"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="C12" s="59" t="s">
+      <c r="A12" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="D12" s="36" t="n">
-        <v>32</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="F12" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="G12" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" s="59" t="s">
-        <v>175</v>
-      </c>
-      <c r="I12" s="60" t="s">
+      <c r="B12" s="0"/>
+      <c r="C12" s="46" t="s">
         <v>202</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="E12" s="0"/>
+      <c r="F12" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0" t="s">
+        <v>203</v>
       </c>
       <c r="J12" s="61"/>
       <c r="K12" s="61"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="C13" s="59" t="s">
+      <c r="A13" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="D13" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="E13" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="F13" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="G13" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="I13" s="59" t="s">
-        <v>182</v>
+      <c r="B13" s="0"/>
+      <c r="C13" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0"/>
+      <c r="F13" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0" t="s">
+        <v>206</v>
       </c>
       <c r="J13" s="61"/>
       <c r="K13" s="61"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="C14" s="59" t="s">
-        <v>206</v>
-      </c>
-      <c r="D14" s="36" t="n">
-        <v>11</v>
-      </c>
-      <c r="F14" s="59" t="s">
+      <c r="A14" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="G14" s="59" t="s">
-        <v>207</v>
-      </c>
-      <c r="I14" s="25" t="s">
+      <c r="B14" s="0"/>
+      <c r="C14" s="46" t="s">
         <v>208</v>
       </c>
+      <c r="D14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E14" s="0"/>
+      <c r="F14" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" s="0"/>
+      <c r="C15" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E15" s="0"/>
+      <c r="F15" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="C15" s="59" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" s="36" t="n">
-        <v>32</v>
-      </c>
-      <c r="F15" s="59" t="s">
-        <v>207</v>
-      </c>
-      <c r="G15" s="59" t="s">
-        <v>207</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>211</v>
+      <c r="G15" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="46" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="46" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G16" s="46" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H16" s="0"/>
       <c r="I16" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
@@ -3494,25 +3570,25 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B17" s="0"/>
       <c r="C17" s="46" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="E17" s="0"/>
       <c r="F17" s="46" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G17" s="46" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J17" s="0"/>
       <c r="K17" s="0"/>
@@ -3521,25 +3597,25 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="46" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E18" s="0"/>
       <c r="F18" s="46" t="s">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="H18" s="0"/>
       <c r="I18" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
@@ -3548,112 +3624,35 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B19" s="0"/>
       <c r="C19" s="46" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E19" s="0"/>
       <c r="F19" s="46" t="s">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="G19" s="46" t="s">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="H19" s="0"/>
       <c r="I19" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="B20" s="0"/>
-      <c r="C20" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="E20" s="0"/>
-      <c r="F20" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="G20" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="H20" s="0"/>
-      <c r="I20" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="J20" s="0"/>
-      <c r="K20" s="0"/>
-      <c r="L20" s="0"/>
-      <c r="M20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="B21" s="0"/>
-      <c r="C21" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="E21" s="0"/>
-      <c r="F21" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="G21" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="H21" s="0"/>
-      <c r="I21" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="J21" s="0"/>
-      <c r="K21" s="0"/>
-      <c r="L21" s="0"/>
-      <c r="M21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B22" s="0"/>
-      <c r="C22" s="46" t="s">
-        <v>232</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E22" s="0"/>
-      <c r="F22" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="G22" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="H22" s="0"/>
-      <c r="I22" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="J22" s="0"/>
-      <c r="K22" s="0"/>
-      <c r="L22" s="0"/>
-      <c r="M22" s="0"/>
-    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1" type="list">
@@ -3676,12 +3675,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3699,13 +3698,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
@@ -3725,7 +3724,7 @@
     </row>
     <row r="2" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B2" s="59" t="s">
         <v>169</v>
@@ -3746,12 +3745,12 @@
         <v>170</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="65" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B3" s="59" t="s">
         <v>174</v>
@@ -3772,12 +3771,12 @@
         <v>170</v>
       </c>
       <c r="H3" s="67" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="65" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>177</v>
@@ -3798,12 +3797,12 @@
         <v>170</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="65" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>177</v>
@@ -3821,15 +3820,15 @@
         <v>172</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H5" s="67" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>177</v>
@@ -3850,12 +3849,12 @@
         <v>170</v>
       </c>
       <c r="H6" s="67" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>177</v>
@@ -3867,21 +3866,21 @@
         <v>1</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G7" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H7" s="67" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>177</v>
@@ -3893,16 +3892,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F8" s="44" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G8" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H8" s="67" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3933,7 +3932,7 @@
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>183</v>
@@ -3954,12 +3953,12 @@
         <v>170</v>
       </c>
       <c r="H10" s="67" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B11" s="59" t="s">
         <v>186</v>
@@ -3980,12 +3979,12 @@
         <v>170</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>189</v>
@@ -4006,12 +4005,12 @@
         <v>170</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="65" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>189</v>
@@ -4029,15 +4028,15 @@
         <v>172</v>
       </c>
       <c r="G13" s="66" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>189</v>
@@ -4058,12 +4057,12 @@
         <v>170</v>
       </c>
       <c r="H14" s="67" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="65" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>189</v>
@@ -4075,21 +4074,21 @@
         <v>1</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G15" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H15" s="67" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B16" s="59" t="s">
         <v>189</v>
@@ -4101,16 +4100,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G16" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H16" s="67" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4141,10 +4140,10 @@
     </row>
     <row r="18" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B18" s="59" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C18" s="44" t="n">
         <v>0</v>
@@ -4153,24 +4152,24 @@
         <v>2</v>
       </c>
       <c r="E18" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F18" s="44" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G18" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H18" s="67" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C19" s="44" t="n">
         <v>8</v>
@@ -4179,25 +4178,25 @@
         <v>6</v>
       </c>
       <c r="E19" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G19" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H19" s="67" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="J19" s="67"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C20" s="44" t="n">
         <v>0</v>
@@ -4206,24 +4205,24 @@
         <v>32</v>
       </c>
       <c r="E20" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F20" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G20" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H20" s="67" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="65" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C21" s="44" t="n">
         <v>0</v>
@@ -4232,24 +4231,24 @@
         <v>1</v>
       </c>
       <c r="E21" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F21" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G21" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H21" s="67" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C22" s="44" t="n">
         <v>1</v>
@@ -4258,24 +4257,24 @@
         <v>1</v>
       </c>
       <c r="E22" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F22" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G22" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H22" s="67" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="65" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C23" s="44" t="n">
         <v>2</v>
@@ -4284,24 +4283,24 @@
         <v>1</v>
       </c>
       <c r="E23" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F23" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G23" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H23" s="67" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="65" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B24" s="59" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C24" s="44" t="n">
         <v>8</v>
@@ -4310,24 +4309,24 @@
         <v>8</v>
       </c>
       <c r="E24" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F24" s="44" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G24" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H24" s="67" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="65" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C25" s="46" t="n">
         <v>16</v>
@@ -4336,24 +4335,24 @@
         <v>10</v>
       </c>
       <c r="E25" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F25" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G25" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H25" s="60" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="65" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C26" s="46" t="n">
         <v>0</v>
@@ -4362,24 +4361,24 @@
         <v>1</v>
       </c>
       <c r="E26" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F26" s="59" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="G26" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H26" s="60" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C27" s="46" t="n">
         <v>0</v>
@@ -4388,24 +4387,24 @@
         <v>32</v>
       </c>
       <c r="E27" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F27" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G27" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H27" s="60" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C28" s="46" t="n">
         <v>0</v>
@@ -4414,24 +4413,24 @@
         <v>32</v>
       </c>
       <c r="E28" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F28" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G28" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H28" s="60" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C29" s="46" t="n">
         <v>0</v>
@@ -4440,24 +4439,24 @@
         <v>32</v>
       </c>
       <c r="E29" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F29" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G29" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H29" s="60" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C30" s="46" t="n">
         <v>0</v>
@@ -4466,15 +4465,119 @@
         <v>32</v>
       </c>
       <c r="E30" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F30" s="66" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="G30" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H30" s="60" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="66" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="H31" s="60" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="C32" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" s="60" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="46" t="n">
+        <v>16</v>
+      </c>
+      <c r="D33" s="46" t="n">
+        <v>6</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="H33" s="60" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B34" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="C34" s="44" t="n">
+        <v>24</v>
+      </c>
+      <c r="D34" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E34" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="F34" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="H34" s="60" t="s">
         <v>275</v>
       </c>
     </row>
@@ -4517,13 +4620,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="68" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
@@ -4630,7 +4733,7 @@
         <v>276</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
DOC:     + Add a basic programmer manual with all the main commands (init, read, write, multi bloc r/w)     + Add the procedure in reference xlsx
</commit_message>
<xml_diff>
--- a/doc/SDIO_reference.xlsx
+++ b/doc/SDIO_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,8 @@
     <sheet name="IPTREGMAP_rel1.0.0" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="IPUDMACMDLIST_rel1.0.0" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="IPUDMACMDMAP_rel1.0.0" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="IPTESTPLAN_rel1.0.0" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="IP_Program_Guide" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="IPTESTPLAN_rel1.0.0" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="IF_DIR" vbProcedure="false">#REF!</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="327">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -909,6 +910,208 @@
     <t xml:space="preserve">EOT</t>
   </si>
   <si>
+    <t xml:space="preserve">Indicate the end of the transfer of  command or data :
+-1'b0: not end
+-1'b1: end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicate the error of the transfer of  command or data :
+-1'b0: no error
+-1'b1: error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_ERR_STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicate the error status of the transfer of  command :
+-6’b00000: no error
+-6'b00001: Response Time Out
+-6'b00010: Response Wrong Direction
+-6'b00100: Response Busy Timeout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA_ERR_STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicate the error status of the transfer of  data :
+-6’b00000: no error
+-6'b00001: Response Time Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Command Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter Bit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UDMA_GC-&gt;CG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1A102000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOCEU-&gt;FC_MASK[8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1A106004 – 0x1A106024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Start/Stop IP clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear UDMA clock gating register bit 9 for SDIO  = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP has the clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set UDMA clock gating register bit 9 for SDIO = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP has no clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Enable or disable IP interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clear SoC event unit FC interrupt mask SDIO’s events’ index  = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP’s interrupt can go to microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set SoC event unit FC interrupt mask SDIO’s events’ index  = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP’s interrupt can not go to microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Frequency control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set CLKDIV  to the number wanted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP’s frequency = Perpheral frequency / (CLKDIV*2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must after operation 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. SDIO RX TX enable control </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set  TX_ENA = 1 and RX_ENA = 1 to enable RX and TX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP enable RX TX according to setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. SDIO init procedure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEND CMD0 and wait for EOT (polling or interrupt)
+SEND CMD8 to check  voltage range
+    If timeout → use default voltage
+    Else check if voltage range is compatible with host (card unusable otherwise)
+SEND CMD55 and ACMD41 in a loop while device returns BUSY
+   CMD55 has no argument
+   ACMD41 with arg=0 → standard capacity card (2G)
+   ACMD41 with arg=1 → high capacitiy card (up to 32G)
+SEND CMD2 → returns 128 bits CID, which can be ignored
+SEND CMD3 → returns RCA in RSP0 register (bits [31:16])
+    RCA will be needed for transfers and should be stored 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end card, is in idle (power on) state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must after operation 1, 4, 2 if want irq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Select and configure card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEND CMD7 with previsouvly obtained RCA
+SEND CMD55+ACMD6 with arg either 0 for single mode or 2 for quad mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end card is in data ready state
+Data transfer mode is set to either quad or single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must come after operation 1,4,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Send data (one block)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocate L2 tranfer buffer
+Set SETUP TX_ENA = 1
+Set TX_SADDR = buffer start pointer address
+Set TX_SIZE       =  buffer size → should multiple of BLOCK SIZE (512)
+Set TX_CFG  register EN bit = 1
+Set SDIO→SETUP register with: 
+    BLOCK_NUM = 0 (NB_BLOCKs-1)
+    RWN = 0; BLOCK_SIZE = 511 (512-1); DATA_EN = 1
+   quad to 1 if chosen quad mode during step 6, 0 otherwise
+SEND CMD24 with sd address as argument
+Wait IP transfer finished (IRQ or polling on SDIO-&gt;STATUS)
+Check STATUS to see if there is error/timeout or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+IP start to transfer data, busy
+SDIO-&gt;STATUS  register EOT bit = 0 , Transfer finished
+SDIO→STATUS register TIMEOUT =1, CMD timeout
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Must after operation 1, 5, 6, 2 if want irq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Receive data (one block)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocate L2 receive buffer
+Set SETUP RX_ENA = 1
+Set RX_SADDR = buffer start pointer address
+Set RX_SIZE       =  buffer size → should multiple of BLOCK SIZE (512)
+Set RX_CFG  register EN bit = 1
+Set SDIO→SETUP register with: 
+    BLOCK_NUM = 0 (NB_BLOCKs-1)
+    RWN = 1; BLOCK_SIZE = 511 (512-1); DATA_EN = 1
+   quad to 1 if chosen quad mode during step 6, 0 otherwise
+SEND CMD17 with sd address as argument
+Wait IP transfer finished (IRQ or polling on SDIO-&gt;STATUS)
+Check STATUS to see if there is error/timeout or not</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -917,7 +1120,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Indicate the end of the transfer of  command or data :
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -927,104 +1130,45 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">-1'b0: not end
--1'b1: end</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">ERROR</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Indicate the error of the transfer of  command or data :
+      <t xml:space="preserve">IP start to transfer data, busy
+SDIO-&gt;STATUS  register EOT bit = 0 , Transfer finished
+SDIO→STATUS register TIMEOUT =1, CMD timeout
 </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-1'b0: no error
--1'b1: error</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">CMD_ERR_STATUS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Indicate the error status of the transfer of  command :
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-6’b00000: no error
--6'b00001: Response Time Out
--6'b00010: Response Wrong Direction
--6'b00100: Response Busy Timeout</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">DATA_ERR_STATUS</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Indicate the error status of the transfer of  data :
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-6’b00000: no error
--6'b00001: Response Time Out</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Command name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Command Field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter Bit field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7b. Send data (multi block)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocate L2 tranfer buffer
+Set SETUP TX_ENA = 1
+Set TX_SADDR = buffer start pointer address
+Set TX_SIZE       =  buffer size → should multiple of BLOCK SIZE (512)
+Set TX_CFG  register EN bit = 1
+Set SDIO→SETUP register with: 
+    BLOCK_NUM = NB_BLOCKs-1
+    RWN = 0; BLOCK_SIZE = 511 (512-1); DATA_EN = 1
+   quad to 1 if chosen quad mode during step 6, 0 otherwise
+SEND CMD25 with sd address as argument
+Wait IP transfer finished (IRQ or polling on SDIO-&gt;STATUS)
+Check STATUS to see if there is error/timeout or not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8b. Receive data (multi block)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocate L2 receive buffer
+Set SETUP RX_ENA = 1
+Set RX_SADDR = buffer start pointer address
+Set RX_SIZE       =  buffer size → should multiple of BLOCK SIZE (512)
+Set RX_CFG  register EN bit = 1
+Set SDIO→SETUP register with: 
+    BLOCK_NUM = NB_BLOCKs-1
+    RWN = 1; BLOCK_SIZE = 511 (512-1); DATA_EN = 1
+   quad to 1 if chosen quad mode during step 6, 0 otherwise
+SEND CMD18 with sd address as argument
+Wait IP transfer finished (IRQ or polling on SDIO-&gt;STATUS)
+Check STATUS to see if there is error/timeout or not</t>
   </si>
   <si>
     <t xml:space="preserve">test ID</t>
@@ -1040,7 +1184,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1090,6 +1234,14 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1248,7 +1400,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1522,6 +1674,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1875,9 +2043,244 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.15"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="45"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="70" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="70" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65" t="s">
+        <v>299</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>300</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>301</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>304</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>305</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="65"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+    </row>
+    <row r="18" customFormat="false" ht="158.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="65" t="s">
+        <v>306</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>307</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>308</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="65" t="s">
+        <v>310</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="60" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="176.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="65" t="s">
+        <v>314</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>315</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>316</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="160.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="65" t="s">
+        <v>318</v>
+      </c>
+      <c r="B21" s="71" t="s">
+        <v>319</v>
+      </c>
+      <c r="C21" s="60" t="s">
+        <v>320</v>
+      </c>
+      <c r="D21" s="72" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="65" t="s">
+        <v>321</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" s="60" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="65" t="s">
+        <v>323</v>
+      </c>
+      <c r="B23" s="71" t="s">
+        <v>324</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>320</v>
+      </c>
+      <c r="D23" s="72" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:C6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1891,10 +2294,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45" t="s">
-        <v>281</v>
+        <v>325</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>282</v>
+        <v>326</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>11</v>
@@ -3677,7 +4080,7 @@
   </sheetPr>
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
@@ -4708,7 +5111,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -4745,6 +5148,7 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Doc:     + Update commands doc
</commit_message>
<xml_diff>
--- a/doc/SDIO_reference.xlsx
+++ b/doc/SDIO_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="383">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -669,6 +669,9 @@
     <t xml:space="preserve">W</t>
   </si>
   <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
     <t xml:space="preserve">SDIO command</t>
   </si>
   <si>
@@ -705,9 +708,6 @@
     <t xml:space="preserve">0x30</t>
   </si>
   <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
     <t xml:space="preserve">Response byte0</t>
   </si>
   <si>
@@ -754,6 +754,24 @@
   </si>
   <si>
     <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_STOPCMD_OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO STOP command op</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO_STOPCMD_ARG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO STOP command arg</t>
   </si>
   <si>
     <t xml:space="preserve">Bit field</t>
@@ -837,7 +855,7 @@
     <t xml:space="preserve">CMD_RSP_TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">Response Type:
+    <t xml:space="preserve">Response type:
 -3’b000: No Responce
 -3’b001: 48 bits with CRC
 -3’b010: 48 bits no CRC
@@ -941,19 +959,177 @@
 -6'b00001: Response Time Out</t>
   </si>
   <si>
+    <t xml:space="preserve">STOPCMD_OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO STOP command opcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOPCMD_RSP_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDIO STOP command response type:
+-3’b000: No Responce
+-3’b001: 48 bits with CRC
+-3’b010: 48 bits no CRC
+-3’b011: 136bits
+-3’b100: 48 bits with BUSY check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOPCMD_ARG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argument to be sent with the STOP command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLK_DIV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock diviser</t>
+  </si>
+  <si>
     <t xml:space="preserve">Command name</t>
   </si>
   <si>
-    <t xml:space="preserve">Command Field</t>
+    <t xml:space="preserve">Command field</t>
   </si>
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
   <si>
-    <t xml:space="preserve">Parameter Bit field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Field Value</t>
+    <t xml:space="preserve">CMD_GO_IDLE_STATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerup or reset card to idle state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_SEND_CID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instruct all cards to send CID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_SEND_RCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instruct all cards to send RCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_SEND_VOLTAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host voltage range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send host voltage configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_APP_SPEC_CMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signal next command is a specific command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACMD_HCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacity mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send host capacity support (high or standard capacity) and ask device for its voltage window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_SELECT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select one card with its RCA and flip READY state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACMD_CFG_QUAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb data lanes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configure the number of lines to use (single or quad mode)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_READ_SINGLE_BLOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">device address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask the device for one single block of data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_READ_MULT_BLOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ask the device to continuously send blocks of data until it receives stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_WRITE_SINGLE_BLOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write a single block of data to the device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_WRITE_MULT_BLOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write a continuous stream of data blocks to device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_SD_STOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP command for sd cards, stop multi block transfers after current block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter bit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMD_RSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X1</t>
   </si>
   <si>
     <t xml:space="preserve">UDMA_GC-&gt;CG</t>
@@ -1112,31 +1288,6 @@
 Check STATUS to see if there is error/timeout or not</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">IP start to transfer data, busy
-SDIO-&gt;STATUS  register EOT bit = 0 , Transfer finished
-SDIO→STATUS register TIMEOUT =1, CMD timeout
-</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">7b. Send data (multi block)</t>
   </si>
   <si>
@@ -1184,7 +1335,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1244,12 +1395,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1400,7 +1545,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="71">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1683,14 +1828,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2045,7 +2182,7 @@
   </sheetPr>
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -2055,30 +2192,31 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>281</v>
+        <v>338</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>282</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>283</v>
+        <v>340</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>284</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="45" t="s">
-        <v>285</v>
+        <v>342</v>
       </c>
       <c r="B6" s="69" t="s">
         <v>11</v>
@@ -2088,67 +2226,67 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="70" t="s">
-        <v>286</v>
+        <v>343</v>
       </c>
       <c r="C7" s="70" t="s">
-        <v>287</v>
+        <v>344</v>
       </c>
       <c r="D7" s="70" t="s">
-        <v>288</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>289</v>
+        <v>346</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>290</v>
+        <v>347</v>
       </c>
       <c r="C8" s="55" t="s">
-        <v>291</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>292</v>
+        <v>349</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>293</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>294</v>
+        <v>351</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>295</v>
+        <v>352</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>296</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>297</v>
+        <v>354</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>298</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>299</v>
+        <v>356</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>300</v>
+        <v>357</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>301</v>
+        <v>358</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>302</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2158,16 +2296,16 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>303</v>
+        <v>360</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>304</v>
+        <v>361</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>305</v>
+        <v>362</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>302</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,86 +2315,86 @@
     </row>
     <row r="18" customFormat="false" ht="158.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
       <c r="B18" s="60" t="s">
-        <v>307</v>
+        <v>364</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>308</v>
+        <v>365</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>309</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
-        <v>310</v>
+        <v>367</v>
       </c>
       <c r="B19" s="60" t="s">
-        <v>311</v>
+        <v>368</v>
       </c>
       <c r="C19" s="60" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="176.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>314</v>
+        <v>371</v>
       </c>
       <c r="B20" s="60" t="s">
-        <v>315</v>
+        <v>372</v>
       </c>
       <c r="C20" s="60" t="s">
-        <v>316</v>
+        <v>373</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>317</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="160.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="65" t="s">
-        <v>318</v>
-      </c>
-      <c r="B21" s="71" t="s">
-        <v>319</v>
+        <v>375</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>376</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>320</v>
-      </c>
-      <c r="D21" s="72" t="s">
-        <v>317</v>
+        <v>373</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>321</v>
+        <v>377</v>
       </c>
       <c r="B22" s="60" t="s">
-        <v>322</v>
+        <v>378</v>
       </c>
       <c r="C22" s="60" t="s">
-        <v>316</v>
+        <v>373</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>317</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="65" t="s">
-        <v>323</v>
-      </c>
-      <c r="B23" s="71" t="s">
-        <v>324</v>
+        <v>379</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>380</v>
       </c>
       <c r="C23" s="60" t="s">
-        <v>320</v>
-      </c>
-      <c r="D23" s="72" t="s">
-        <v>317</v>
+        <v>373</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -2294,10 +2432,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="45" t="s">
-        <v>325</v>
+        <v>381</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>326</v>
+        <v>382</v>
       </c>
       <c r="C1" s="45" t="s">
         <v>11</v>
@@ -3524,19 +3662,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="18.49"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="36" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="36" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="4.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="36" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="25" width="46.12"/>
@@ -3812,26 +3949,26 @@
         <v>195</v>
       </c>
       <c r="D10" s="36" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F10" s="59" t="s">
         <v>196</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J10" s="61"/>
       <c r="K10" s="61"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="36" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D11" s="36" t="n">
         <v>32</v>
@@ -3840,21 +3977,21 @@
         <v>196</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J11" s="61"/>
       <c r="K11" s="61"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="46" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>26</v>
@@ -3868,18 +4005,18 @@
       </c>
       <c r="H12" s="0"/>
       <c r="I12" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J12" s="61"/>
       <c r="K12" s="61"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B13" s="0"/>
       <c r="C13" s="46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -3893,28 +4030,28 @@
       </c>
       <c r="H13" s="0"/>
       <c r="I13" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J13" s="61"/>
       <c r="K13" s="61"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B14" s="0"/>
       <c r="C14" s="46" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E14" s="0"/>
       <c r="F14" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G14" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H14" s="0"/>
       <c r="I14" s="0" t="s">
@@ -3934,10 +4071,10 @@
       </c>
       <c r="E15" s="0"/>
       <c r="F15" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G15" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H15" s="0"/>
       <c r="I15" s="0" t="s">
@@ -3957,10 +4094,10 @@
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G16" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H16" s="0"/>
       <c r="I16" s="0" t="s">
@@ -3984,10 +4121,10 @@
       </c>
       <c r="E17" s="0"/>
       <c r="F17" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G17" s="46" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="H17" s="0"/>
       <c r="I17" s="0" t="s">
@@ -4052,8 +4189,52 @@
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" s="36" t="n">
+        <v>14</v>
+      </c>
+      <c r="F20" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="C21" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D21" s="36" t="n">
+        <v>32</v>
+      </c>
+      <c r="F21" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="G21" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4078,17 +4259,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
@@ -4101,13 +4282,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
@@ -4127,7 +4308,7 @@
     </row>
     <row r="2" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="65" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B2" s="59" t="s">
         <v>169</v>
@@ -4148,12 +4329,12 @@
         <v>170</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="65" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B3" s="59" t="s">
         <v>174</v>
@@ -4174,12 +4355,12 @@
         <v>170</v>
       </c>
       <c r="H3" s="67" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="65" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>177</v>
@@ -4200,12 +4381,12 @@
         <v>170</v>
       </c>
       <c r="H4" s="67" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="65" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>177</v>
@@ -4223,15 +4404,15 @@
         <v>172</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="H5" s="67" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="65" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>177</v>
@@ -4252,18 +4433,18 @@
         <v>170</v>
       </c>
       <c r="H6" s="67" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="65" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>177</v>
       </c>
       <c r="C7" s="44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7" s="44" t="n">
         <v>1</v>
@@ -4272,18 +4453,18 @@
         <v>196</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G7" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H7" s="67" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="65" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>177</v>
@@ -4295,7 +4476,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F8" s="44" t="s">
         <v>196</v>
@@ -4304,7 +4485,7 @@
         <v>170</v>
       </c>
       <c r="H8" s="67" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4335,7 +4516,7 @@
     </row>
     <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="65" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>183</v>
@@ -4356,12 +4537,12 @@
         <v>170</v>
       </c>
       <c r="H10" s="67" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="65" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B11" s="59" t="s">
         <v>186</v>
@@ -4382,12 +4563,12 @@
         <v>170</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="65" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>189</v>
@@ -4408,12 +4589,12 @@
         <v>170</v>
       </c>
       <c r="H12" s="67" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="65" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>189</v>
@@ -4431,15 +4612,15 @@
         <v>172</v>
       </c>
       <c r="G13" s="66" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="65" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>189</v>
@@ -4460,18 +4641,18 @@
         <v>170</v>
       </c>
       <c r="H14" s="67" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="65" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>189</v>
       </c>
       <c r="C15" s="44" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="44" t="n">
         <v>1</v>
@@ -4480,18 +4661,18 @@
         <v>196</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G15" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H15" s="67" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="65" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B16" s="59" t="s">
         <v>189</v>
@@ -4503,7 +4684,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F16" s="44" t="s">
         <v>196</v>
@@ -4512,7 +4693,7 @@
         <v>170</v>
       </c>
       <c r="H16" s="67" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4543,7 +4724,7 @@
     </row>
     <row r="18" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="B18" s="59" t="s">
         <v>194</v>
@@ -4552,7 +4733,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="44" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="59" t="s">
         <v>196</v>
@@ -4564,12 +4745,12 @@
         <v>170</v>
       </c>
       <c r="H18" s="67" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="65" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="B19" s="59" t="s">
         <v>194</v>
@@ -4584,22 +4765,22 @@
         <v>196</v>
       </c>
       <c r="F19" s="59" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G19" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H19" s="67" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="J19" s="67"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="65" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B20" s="59" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C20" s="44" t="n">
         <v>0</v>
@@ -4611,21 +4792,21 @@
         <v>196</v>
       </c>
       <c r="F20" s="59" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G20" s="66" t="s">
         <v>170</v>
       </c>
       <c r="H20" s="67" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="65" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C21" s="44" t="n">
         <v>0</v>
@@ -4643,15 +4824,15 @@
         <v>170</v>
       </c>
       <c r="H21" s="67" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="65" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B22" s="59" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C22" s="44" t="n">
         <v>1</v>
@@ -4669,15 +4850,15 @@
         <v>170</v>
       </c>
       <c r="H22" s="67" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="65" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="B23" s="59" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C23" s="44" t="n">
         <v>2</v>
@@ -4695,15 +4876,15 @@
         <v>170</v>
       </c>
       <c r="H23" s="67" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="65" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B24" s="59" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C24" s="44" t="n">
         <v>8</v>
@@ -4721,15 +4902,15 @@
         <v>170</v>
       </c>
       <c r="H24" s="67" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="65" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C25" s="46" t="n">
         <v>16</v>
@@ -4747,15 +4928,15 @@
         <v>170</v>
       </c>
       <c r="H25" s="60" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="65" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C26" s="46" t="n">
         <v>0</v>
@@ -4773,15 +4954,15 @@
         <v>170</v>
       </c>
       <c r="H26" s="60" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C27" s="46" t="n">
         <v>0</v>
@@ -4790,16 +4971,16 @@
         <v>32</v>
       </c>
       <c r="E27" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F27" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G27" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H27" s="60" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4816,16 +4997,16 @@
         <v>32</v>
       </c>
       <c r="E28" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F28" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G28" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H28" s="60" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,16 +5023,16 @@
         <v>32</v>
       </c>
       <c r="E29" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F29" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G29" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H29" s="60" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4868,21 +5049,21 @@
         <v>32</v>
       </c>
       <c r="E30" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F30" s="66" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G30" s="46" t="s">
         <v>170</v>
       </c>
       <c r="H30" s="60" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>223</v>
@@ -4903,12 +5084,12 @@
         <v>170</v>
       </c>
       <c r="H31" s="60" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>223</v>
@@ -4929,12 +5110,12 @@
         <v>170</v>
       </c>
       <c r="H32" s="60" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="53.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>223</v>
@@ -4946,21 +5127,21 @@
         <v>6</v>
       </c>
       <c r="E33" s="44" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F33" s="44" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G33" s="44" t="s">
         <v>170</v>
       </c>
       <c r="H33" s="60" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>223</v>
@@ -4972,18 +5153,123 @@
         <v>6</v>
       </c>
       <c r="E34" s="44" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F34" s="44" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G34" s="44" t="s">
         <v>170</v>
       </c>
       <c r="H34" s="60" t="s">
-        <v>275</v>
-      </c>
-    </row>
+        <v>281</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="35" t="s">
+        <v>282</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="C35" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D35" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E35" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="G35" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="H35" s="67" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="B36" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="C36" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="G36" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="67" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="44" t="n">
+        <v>32</v>
+      </c>
+      <c r="E37" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="F37" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="G37" s="66" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="67" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="B38" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="44" t="n">
+        <v>9</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="G38" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="H38" s="62" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5023,13 +5309,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="68" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
@@ -5063,15 +5349,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="15.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="44" width="17.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="76.81"/>
@@ -5080,19 +5366,240 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="68" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>78</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="E1" s="68" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="55" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B4" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B5" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B8" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B9" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B10" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B13" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>328</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B14" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -5111,16 +5618,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="26.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="11.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="13.09"/>
@@ -5130,25 +5637,468 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="64" t="s">
-        <v>279</v>
+        <v>333</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>228</v>
+        <v>104</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>78</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>280</v>
+        <v>334</v>
       </c>
       <c r="F1" s="68" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="C2" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="C6" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D6" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B12" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B13" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="C13" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="C14" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="C15" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="C16" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D16" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="C18" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D18" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>319</v>
+      </c>
+      <c r="C19" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="C20" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>323</v>
+      </c>
+      <c r="C21" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="C22" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D22" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="C23" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E23" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="C24" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D24" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B25" s="46" t="s">
+        <v>327</v>
+      </c>
+      <c r="C25" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="65" t="s">
+        <v>254</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="C26" s="44" t="n">
+        <v>8</v>
+      </c>
+      <c r="D26" s="44" t="n">
+        <v>6</v>
+      </c>
+      <c r="E26" s="44" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>330</v>
+      </c>
+      <c r="C27" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="44" t="n">
+        <v>3</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>